<commit_message>
GUI from debug to release. Fixed data not imported bug
</commit_message>
<xml_diff>
--- a/Prod_Plan_Manual.xlsx
+++ b/Prod_Plan_Manual.xlsx
@@ -14,15 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Machine</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Machines</t>
+  </si>
+  <si>
+    <t>Order 3 - 26</t>
+  </si>
+  <si>
+    <t>Order 6 - 52</t>
+  </si>
+  <si>
+    <t>Order 7 - 109</t>
+  </si>
+  <si>
+    <t>Order 4 - 129</t>
   </si>
   <si>
     <t>Order 5 - 40</t>
   </si>
   <si>
-    <t>make span: 40</t>
+    <t>Order 8 - 74</t>
+  </si>
+  <si>
+    <t>Order 1 - 135</t>
+  </si>
+  <si>
+    <t>Order 9 - 183</t>
+  </si>
+  <si>
+    <t>Order 2 - 222</t>
+  </si>
+  <si>
+    <t>Order 10 - 70</t>
+  </si>
+  <si>
+    <t>make span: 222</t>
   </si>
 </sst>
 </file>
@@ -362,19 +389,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:D6"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -383,8 +410,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>222</v>
+      </c>
+      <c r="B4">
+        <v>93</v>
+      </c>
       <c r="C4">
         <v>0</v>
+      </c>
+      <c r="D4">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -402,8 +438,43 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>